<commit_message>
1. NEW UI 2. assign.html added for assignment 3. assignment and end task are now working 4. user task initialized 5. ui form attached 6. pmRegisterForm.html 7.fixes 8.Event is now working(Register, Update, View) 9. users can only update their assigned task details font and design improvement delayCalculation will not count weekends
DailyReport.java initialized

Working on DailyReport, task and event to how they shoud work together. still analyzing
report_event table seems working fine
first demo was successful
division of labour between task and event
</commit_message>
<xml_diff>
--- a/TaskStatus.xlsx
+++ b/TaskStatus.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8567B9BF-73AD-4824-AD1A-A37EF2DF8F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="150">
   <si>
     <t>3.    بررسی فلزات از نظر زنگ زدگی.</t>
   </si>
@@ -474,15 +473,12 @@
   </si>
   <si>
     <t>active</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
@@ -831,12 +827,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +841,9 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
@@ -864,233 +859,260 @@
       <c r="E1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45236</v>
+      </c>
       <c r="D2" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C3" s="4">
+        <v>45018</v>
+      </c>
       <c r="D3" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="1">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45019</v>
+      </c>
       <c r="D4" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>45020</v>
+      </c>
       <c r="D5" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>45021</v>
+      </c>
       <c r="D6" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="1">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C7" s="4">
+        <v>45022</v>
+      </c>
       <c r="D7" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C8" s="4">
+        <v>45023</v>
+      </c>
       <c r="D8" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>121</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>45024</v>
+      </c>
       <c r="D9" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="1">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45025</v>
+      </c>
       <c r="D10" s="4">
-        <v>45248</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45026</v>
+      </c>
       <c r="D11" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45027</v>
+      </c>
       <c r="D12" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="1">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>45028</v>
+      </c>
       <c r="D13" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4">
+        <v>45029</v>
+      </c>
       <c r="D14" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>45030</v>
+      </c>
       <c r="D15" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+        <v>45238</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C16" s="4">
+        <v>45031</v>
+      </c>
       <c r="D16" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
+        <v>45238</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1098,14 +1120,16 @@
         <v>128</v>
       </c>
       <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C17" s="4">
+        <v>45032</v>
+      </c>
       <c r="D17" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1115,12 +1139,14 @@
       <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4">
+        <v>45033</v>
+      </c>
       <c r="D18" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1128,14 +1154,16 @@
         <v>127</v>
       </c>
       <c r="B19" s="1">
-        <v>7</v>
-      </c>
-      <c r="C19" s="4"/>
+        <v>365</v>
+      </c>
+      <c r="C19" s="4">
+        <v>45034</v>
+      </c>
       <c r="D19" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1143,14 +1171,16 @@
         <v>81</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45035</v>
+      </c>
       <c r="D20" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1158,14 +1188,16 @@
         <v>129</v>
       </c>
       <c r="B21" s="1">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C21" s="4">
+        <v>45036</v>
+      </c>
       <c r="D21" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1173,14 +1205,16 @@
         <v>130</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45037</v>
+      </c>
       <c r="D22" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1188,14 +1222,16 @@
         <v>131</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C23" s="4">
+        <v>45038</v>
+      </c>
       <c r="D23" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1203,14 +1239,16 @@
         <v>132</v>
       </c>
       <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C24" s="4">
+        <v>45039</v>
+      </c>
       <c r="D24" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1218,14 +1256,16 @@
         <v>86</v>
       </c>
       <c r="B25" s="1">
-        <v>7</v>
-      </c>
-      <c r="C25" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C25" s="4">
+        <v>45040</v>
+      </c>
       <c r="D25" s="4">
-        <v>45250</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1233,14 +1273,16 @@
         <v>87</v>
       </c>
       <c r="B26" s="1">
-        <v>7</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C26" s="4">
+        <v>45041</v>
+      </c>
       <c r="D26" s="4">
-        <v>45251</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1248,14 +1290,16 @@
         <v>133</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C27" s="4">
+        <v>45042</v>
+      </c>
       <c r="D27" s="4">
-        <v>45252</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1263,14 +1307,16 @@
         <v>134</v>
       </c>
       <c r="B28" s="1">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C28" s="4">
+        <v>45043</v>
+      </c>
       <c r="D28" s="4">
-        <v>45253</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1280,12 +1326,14 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4">
+        <v>45044</v>
+      </c>
       <c r="D29" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1295,12 +1343,14 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4">
+        <v>45045</v>
+      </c>
       <c r="D30" s="4">
-        <v>45255</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1310,12 +1360,14 @@
       <c r="B31" s="1">
         <v>7</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4">
+        <v>45046</v>
+      </c>
       <c r="D31" s="4">
-        <v>45256</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
+        <v>45239</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1325,12 +1377,14 @@
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4">
+        <v>45047</v>
+      </c>
       <c r="D32" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1340,12 +1394,14 @@
       <c r="B33" s="1">
         <v>7</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4">
+        <v>45048</v>
+      </c>
       <c r="D33" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1355,12 +1411,14 @@
       <c r="B34" s="1">
         <v>7</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="4">
+        <v>45049</v>
+      </c>
       <c r="D34" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1370,12 +1428,14 @@
       <c r="B35" s="1">
         <v>7</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4">
+        <v>45050</v>
+      </c>
       <c r="D35" s="4">
-        <v>45250</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1385,12 +1445,14 @@
       <c r="B36" s="1">
         <v>7</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4">
+        <v>45051</v>
+      </c>
       <c r="D36" s="4">
-        <v>45251</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1400,12 +1462,14 @@
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="4">
+        <v>45052</v>
+      </c>
       <c r="D37" s="4">
-        <v>45252</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1413,14 +1477,16 @@
         <v>137</v>
       </c>
       <c r="B38" s="1">
-        <v>3</v>
-      </c>
-      <c r="C38" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C38" s="4">
+        <v>45053</v>
+      </c>
       <c r="D38" s="4">
-        <v>45253</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0</v>
+        <v>45240</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1428,14 +1494,16 @@
         <v>138</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C39" s="4">
+        <v>45054</v>
+      </c>
       <c r="D39" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
+        <v>45241</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1443,14 +1511,16 @@
         <v>139</v>
       </c>
       <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C40" s="4">
+        <v>45055</v>
+      </c>
       <c r="D40" s="4">
-        <v>45255</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
+        <v>45241</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1458,14 +1528,16 @@
         <v>140</v>
       </c>
       <c r="B41" s="1">
-        <v>3</v>
-      </c>
-      <c r="C41" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
+        <v>45056</v>
+      </c>
       <c r="D41" s="4">
-        <v>45256</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
+        <v>45241</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1473,14 +1545,16 @@
         <v>120</v>
       </c>
       <c r="B42" s="1">
-        <v>7</v>
-      </c>
-      <c r="C42" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C42" s="4">
+        <v>45057</v>
+      </c>
       <c r="D42" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
+        <v>45242</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1490,12 +1564,14 @@
       <c r="B43" s="1">
         <v>1</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="4">
+        <v>45058</v>
+      </c>
       <c r="D43" s="4">
-        <v>45249</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
+        <v>45242</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1503,14 +1579,16 @@
         <v>107</v>
       </c>
       <c r="B44" s="1">
-        <v>7</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C44" s="4">
+        <v>45059</v>
+      </c>
       <c r="D44" s="4">
-        <v>45250</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
+        <v>45242</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1518,14 +1596,16 @@
         <v>141</v>
       </c>
       <c r="B45" s="1">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C45" s="4">
+        <v>45060</v>
+      </c>
       <c r="D45" s="4">
-        <v>45251</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
+        <v>45242</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1533,14 +1613,16 @@
         <v>142</v>
       </c>
       <c r="B46" s="1">
-        <v>3</v>
-      </c>
-      <c r="C46" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C46" s="4">
+        <v>45061</v>
+      </c>
       <c r="D46" s="4">
-        <v>45252</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
+        <v>45242</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1548,14 +1630,16 @@
         <v>143</v>
       </c>
       <c r="B47" s="1">
-        <v>1</v>
-      </c>
-      <c r="C47" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C47" s="4">
+        <v>45062</v>
+      </c>
       <c r="D47" s="4">
-        <v>45253</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1563,14 +1647,16 @@
         <v>144</v>
       </c>
       <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C48" s="4">
+        <v>45063</v>
+      </c>
       <c r="D48" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1578,14 +1664,16 @@
         <v>145</v>
       </c>
       <c r="B49" s="1">
-        <v>3</v>
-      </c>
-      <c r="C49" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C49" s="4">
+        <v>45064</v>
+      </c>
       <c r="D49" s="4">
-        <v>45255</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1593,14 +1681,16 @@
         <v>146</v>
       </c>
       <c r="B50" s="1">
-        <v>7</v>
-      </c>
-      <c r="C50" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
+        <v>45065</v>
+      </c>
       <c r="D50" s="4">
-        <v>45256</v>
-      </c>
-      <c r="E50" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1608,14 +1698,16 @@
         <v>147</v>
       </c>
       <c r="B51" s="1">
-        <v>1</v>
-      </c>
-      <c r="C51" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C51" s="4">
+        <v>45066</v>
+      </c>
       <c r="D51" s="4">
-        <v>45250</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1623,14 +1715,16 @@
         <v>115</v>
       </c>
       <c r="B52" s="1">
-        <v>7</v>
-      </c>
-      <c r="C52" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C52" s="4">
+        <v>45067</v>
+      </c>
       <c r="D52" s="4">
-        <v>45251</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1638,14 +1732,16 @@
         <v>148</v>
       </c>
       <c r="B53" s="1">
-        <v>1</v>
-      </c>
-      <c r="C53" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C53" s="4">
+        <v>45068</v>
+      </c>
       <c r="D53" s="4">
-        <v>45252</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1653,14 +1749,16 @@
         <v>117</v>
       </c>
       <c r="B54" s="1">
-        <v>3</v>
-      </c>
-      <c r="C54" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C54" s="4">
+        <v>45069</v>
+      </c>
       <c r="D54" s="4">
-        <v>45253</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1668,25 +1766,27 @@
         <v>118</v>
       </c>
       <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C55" s="4">
+        <v>45070</v>
+      </c>
       <c r="D55" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E55" s="1">
-        <v>0</v>
+        <v>45243</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D55"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView rightToLeft="1" topLeftCell="L49" workbookViewId="0">

</xml_diff>

<commit_message>
Feature Modularization almost complete..
</commit_message>
<xml_diff>
--- a/TaskStatus.xlsx
+++ b/TaskStatus.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B115B-FA96-4332-8FA4-51F9DF14608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
@@ -827,12 +828,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,16 +866,14 @@
         <v>65</v>
       </c>
       <c r="B2" s="1">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4">
-        <v>45236</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -882,16 +881,14 @@
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>90</v>
-      </c>
-      <c r="C3" s="4">
-        <v>45018</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -899,16 +896,14 @@
         <v>67</v>
       </c>
       <c r="B4" s="1">
-        <v>90</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45019</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -916,16 +911,14 @@
         <v>89</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>45020</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -933,16 +926,14 @@
         <v>68</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>45021</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -950,16 +941,14 @@
         <v>69</v>
       </c>
       <c r="B7" s="1">
-        <v>90</v>
-      </c>
-      <c r="C7" s="4">
-        <v>45022</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -967,16 +956,14 @@
         <v>119</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4">
-        <v>45023</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -984,16 +971,14 @@
         <v>121</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>45024</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1001,16 +986,14 @@
         <v>72</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>45025</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1018,16 +1001,14 @@
         <v>123</v>
       </c>
       <c r="B11" s="1">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4">
-        <v>45026</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1035,16 +1016,14 @@
         <v>74</v>
       </c>
       <c r="B12" s="1">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4">
-        <v>45027</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1052,16 +1031,14 @@
         <v>75</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>45028</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1069,16 +1046,14 @@
         <v>122</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>45029</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1088,14 +1063,12 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="4">
-        <v>45030</v>
-      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1103,16 +1076,14 @@
         <v>125</v>
       </c>
       <c r="B16" s="1">
-        <v>180</v>
-      </c>
-      <c r="C16" s="4">
-        <v>45031</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4">
-        <v>45238</v>
+        <v>45254</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1120,16 +1091,14 @@
         <v>128</v>
       </c>
       <c r="B17" s="1">
-        <v>180</v>
-      </c>
-      <c r="C17" s="4">
-        <v>45032</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1137,16 +1106,14 @@
         <v>126</v>
       </c>
       <c r="B18" s="1">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4">
-        <v>45033</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1154,16 +1121,14 @@
         <v>127</v>
       </c>
       <c r="B19" s="1">
-        <v>365</v>
-      </c>
-      <c r="C19" s="4">
-        <v>45034</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1171,16 +1136,14 @@
         <v>81</v>
       </c>
       <c r="B20" s="1">
-        <v>180</v>
-      </c>
-      <c r="C20" s="4">
-        <v>45035</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1188,16 +1151,14 @@
         <v>129</v>
       </c>
       <c r="B21" s="1">
-        <v>90</v>
-      </c>
-      <c r="C21" s="4">
-        <v>45036</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C21" s="4"/>
       <c r="D21" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1205,16 +1166,14 @@
         <v>130</v>
       </c>
       <c r="B22" s="1">
-        <v>90</v>
-      </c>
-      <c r="C22" s="4">
-        <v>45037</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1222,16 +1181,14 @@
         <v>131</v>
       </c>
       <c r="B23" s="1">
-        <v>30</v>
-      </c>
-      <c r="C23" s="4">
-        <v>45038</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C23" s="4"/>
       <c r="D23" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1239,16 +1196,14 @@
         <v>132</v>
       </c>
       <c r="B24" s="1">
-        <v>30</v>
-      </c>
-      <c r="C24" s="4">
-        <v>45039</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1256,16 +1211,14 @@
         <v>86</v>
       </c>
       <c r="B25" s="1">
-        <v>30</v>
-      </c>
-      <c r="C25" s="4">
-        <v>45040</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1273,16 +1226,14 @@
         <v>87</v>
       </c>
       <c r="B26" s="1">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4">
-        <v>45041</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1290,16 +1241,14 @@
         <v>133</v>
       </c>
       <c r="B27" s="1">
-        <v>180</v>
-      </c>
-      <c r="C27" s="4">
-        <v>45042</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1307,16 +1256,14 @@
         <v>134</v>
       </c>
       <c r="B28" s="1">
-        <v>90</v>
-      </c>
-      <c r="C28" s="4">
-        <v>45043</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1324,16 +1271,14 @@
         <v>92</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>45044</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1341,16 +1286,14 @@
         <v>93</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4">
-        <v>45045</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1360,14 +1303,12 @@
       <c r="B31" s="1">
         <v>7</v>
       </c>
-      <c r="C31" s="4">
-        <v>45046</v>
-      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4">
-        <v>45239</v>
+        <v>45254</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1377,14 +1318,12 @@
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="4">
-        <v>45047</v>
-      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1392,16 +1331,14 @@
         <v>96</v>
       </c>
       <c r="B33" s="1">
-        <v>7</v>
-      </c>
-      <c r="C33" s="4">
-        <v>45048</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C33" s="4"/>
       <c r="D33" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1409,16 +1346,14 @@
         <v>136</v>
       </c>
       <c r="B34" s="1">
-        <v>7</v>
-      </c>
-      <c r="C34" s="4">
-        <v>45049</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1428,14 +1363,12 @@
       <c r="B35" s="1">
         <v>7</v>
       </c>
-      <c r="C35" s="4">
-        <v>45050</v>
-      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1445,14 +1378,12 @@
       <c r="B36" s="1">
         <v>7</v>
       </c>
-      <c r="C36" s="4">
-        <v>45051</v>
-      </c>
+      <c r="C36" s="4"/>
       <c r="D36" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1462,14 +1393,12 @@
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="4">
-        <v>45052</v>
-      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1477,16 +1406,14 @@
         <v>137</v>
       </c>
       <c r="B38" s="1">
-        <v>90</v>
-      </c>
-      <c r="C38" s="4">
-        <v>45053</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C38" s="4"/>
       <c r="D38" s="4">
-        <v>45240</v>
+        <v>45254</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1494,16 +1421,14 @@
         <v>138</v>
       </c>
       <c r="B39" s="1">
-        <v>30</v>
-      </c>
-      <c r="C39" s="4">
-        <v>45054</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="4">
-        <v>45241</v>
+        <v>45254</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1513,14 +1438,12 @@
       <c r="B40" s="1">
         <v>30</v>
       </c>
-      <c r="C40" s="4">
-        <v>45055</v>
-      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="4">
-        <v>45241</v>
+        <v>45254</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1530,14 +1453,12 @@
       <c r="B41" s="1">
         <v>1</v>
       </c>
-      <c r="C41" s="4">
-        <v>45056</v>
-      </c>
+      <c r="C41" s="4"/>
       <c r="D41" s="4">
-        <v>45241</v>
+        <v>45254</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1545,16 +1466,14 @@
         <v>120</v>
       </c>
       <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4">
-        <v>45057</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="4">
-        <v>45242</v>
+        <v>45254</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1564,14 +1483,12 @@
       <c r="B43" s="1">
         <v>1</v>
       </c>
-      <c r="C43" s="4">
-        <v>45058</v>
-      </c>
+      <c r="C43" s="4"/>
       <c r="D43" s="4">
-        <v>45242</v>
+        <v>45254</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1579,16 +1496,14 @@
         <v>107</v>
       </c>
       <c r="B44" s="1">
-        <v>30</v>
-      </c>
-      <c r="C44" s="4">
-        <v>45059</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="4">
-        <v>45242</v>
+        <v>45254</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1596,16 +1511,14 @@
         <v>141</v>
       </c>
       <c r="B45" s="1">
-        <v>30</v>
-      </c>
-      <c r="C45" s="4">
-        <v>45060</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="4">
-        <v>45242</v>
+        <v>45255</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1613,16 +1526,14 @@
         <v>142</v>
       </c>
       <c r="B46" s="1">
-        <v>30</v>
-      </c>
-      <c r="C46" s="4">
-        <v>45061</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C46" s="4"/>
       <c r="D46" s="4">
-        <v>45242</v>
+        <v>45255</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1630,16 +1541,14 @@
         <v>143</v>
       </c>
       <c r="B47" s="1">
-        <v>30</v>
-      </c>
-      <c r="C47" s="4">
-        <v>45062</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C47" s="4"/>
       <c r="D47" s="4">
-        <v>45243</v>
+        <v>45255</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1647,16 +1556,14 @@
         <v>144</v>
       </c>
       <c r="B48" s="1">
-        <v>180</v>
-      </c>
-      <c r="C48" s="4">
-        <v>45063</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C48" s="4"/>
       <c r="D48" s="4">
-        <v>45243</v>
+        <v>45255</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1664,16 +1571,14 @@
         <v>145</v>
       </c>
       <c r="B49" s="1">
-        <v>30</v>
-      </c>
-      <c r="C49" s="4">
-        <v>45064</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="4">
-        <v>45243</v>
+        <v>45256</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1681,16 +1586,14 @@
         <v>146</v>
       </c>
       <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="4">
-        <v>45065</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C50" s="4"/>
       <c r="D50" s="4">
-        <v>45243</v>
+        <v>45256</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1698,16 +1601,14 @@
         <v>147</v>
       </c>
       <c r="B51" s="1">
-        <v>30</v>
-      </c>
-      <c r="C51" s="4">
-        <v>45066</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C51" s="4"/>
       <c r="D51" s="4">
-        <v>45243</v>
+        <v>45256</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1715,16 +1616,14 @@
         <v>115</v>
       </c>
       <c r="B52" s="1">
-        <v>30</v>
-      </c>
-      <c r="C52" s="4">
-        <v>45067</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="4">
-        <v>45243</v>
+        <v>45256</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1732,16 +1631,14 @@
         <v>148</v>
       </c>
       <c r="B53" s="1">
-        <v>30</v>
-      </c>
-      <c r="C53" s="4">
-        <v>45068</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C53" s="4"/>
       <c r="D53" s="4">
-        <v>45243</v>
+        <v>45257</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1749,16 +1646,14 @@
         <v>117</v>
       </c>
       <c r="B54" s="1">
-        <v>90</v>
-      </c>
-      <c r="C54" s="4">
-        <v>45069</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C54" s="4"/>
       <c r="D54" s="4">
-        <v>45243</v>
+        <v>45257</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -1766,27 +1661,25 @@
         <v>118</v>
       </c>
       <c r="B55" s="1">
-        <v>30</v>
-      </c>
-      <c r="C55" s="4">
-        <v>45070</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C55" s="4"/>
       <c r="D55" s="4">
-        <v>45243</v>
+        <v>45257</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D55"/>
+  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView rightToLeft="1" topLeftCell="L49" workbookViewId="0">

</xml_diff>